<commit_message>
bv werkt nu wel etc.
</commit_message>
<xml_diff>
--- a/vragen_antwoorden_vijf_dz_plus.xlsx
+++ b/vragen_antwoorden_vijf_dz_plus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10110"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/90320473a3d91f65/R Projects/Beleggersprofiel/shiny_vertaler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{7DD4128A-3640-514A-A7E0-5F2AAB1F81D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE935304-80D7-7D4E-A363-6C52BB58BF79}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{7DD4128A-3640-514A-A7E0-5F2AAB1F81D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{367544FF-B4B5-8048-A0AE-E3B064C89D6D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1040" windowWidth="30240" windowHeight="17720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1040" windowWidth="30240" windowHeight="17720" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Risicoprofiel bepalen - bron" sheetId="18" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3242" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3242" uniqueCount="708">
   <si>
     <t>Minder dan 25%</t>
   </si>
@@ -2181,9 +2181,6 @@
   </si>
   <si>
     <t>The investments of the association are made for a period of more than ten years</t>
-  </si>
-  <si>
-    <t>the main adverse impacts on sustainability factors as mentioned above should be taken into account</t>
   </si>
   <si>
     <t>we are not interested in private investments for the portfolio of the association</t>
@@ -5625,7 +5622,7 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="D41" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D42" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A51" sqref="A51:XFD55"/>
     </sheetView>
   </sheetViews>
@@ -6813,8 +6810,8 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="D26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="D26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -7832,7 +7829,7 @@
         <v>664</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>700</v>
+        <v>637</v>
       </c>
       <c r="E55" s="77">
         <v>0</v>
@@ -7960,10 +7957,10 @@
         <v>506</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E62" s="70">
         <v>0</v>
@@ -7981,10 +7978,10 @@
         <v>506</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E63" s="26">
         <v>0</v>
@@ -13988,7 +13985,7 @@
   </sheetPr>
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+    <sheetView topLeftCell="D34" workbookViewId="0">
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
@@ -15914,13 +15911,13 @@
         <v>563</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E40" s="66">
         <v>2</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -15934,7 +15931,7 @@
         <v>563</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E41" s="66">
         <v>3</v>
@@ -16314,10 +16311,10 @@
         <v>506</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E62" s="70">
         <v>0</v>
@@ -16335,7 +16332,7 @@
         <v>506</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D63" s="26" t="s">
         <v>591</v>
@@ -17556,7 +17553,7 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -18683,10 +18680,10 @@
         <v>506</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E62" s="70">
         <v>0</v>
@@ -18704,7 +18701,7 @@
         <v>506</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D63" s="26" t="s">
         <v>636</v>
@@ -19868,7 +19865,7 @@
   </sheetPr>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="D37" workbookViewId="0">
+    <sheetView topLeftCell="C22" workbookViewId="0">
       <selection activeCell="A48" sqref="A48:XFD52"/>
     </sheetView>
   </sheetViews>
@@ -20553,7 +20550,7 @@
         <v>655</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E37" s="66">
         <v>2</v>
@@ -20574,7 +20571,7 @@
         <v>655</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E38" s="66">
         <v>3</v>
@@ -20960,10 +20957,10 @@
         <v>506</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D59" s="26" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E59" s="70">
         <v>0</v>
@@ -20981,7 +20978,7 @@
         <v>506</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D60" s="26" t="s">
         <v>670</v>

</xml_diff>